<commit_message>
Disabling Carbon Tax Border Adjustment boolean
CTBA boolean was causing differences in IO between BAU scenario and no settings policy scenario. should consider further review of differences
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BDCTBA/Boolean Disable Carbon Tax Border Adjustment.xlsx
+++ b/InputData/ctrl-settings/BDCTBA/Boolean Disable Carbon Tax Border Adjustment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\ctrl-settings\BDCTBA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire Trevisan\Dropbox (Energy Innovation)\Documents\GitHub\eps-eu\InputData\ctrl-settings\BDCTBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8D7FAB-775F-4521-B28A-D5E0C5AF6AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909ECFB3-35FC-4244-853D-B3FA7B730A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59685" yWindow="1605" windowWidth="21585" windowHeight="12525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -47,10 +47,10 @@
     <t>industries.</t>
   </si>
   <si>
-    <t>Diable Carbon Tax Border Adjustment</t>
-  </si>
-  <si>
     <t>By default, the EPS assumes carbon tax border adjustments do not apply across</t>
+  </si>
+  <si>
+    <t>Disable Carbon Tax Border Adjustment</t>
   </si>
 </sst>
 </file>
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -475,7 +475,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
@@ -496,15 +496,15 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -512,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further WebAppData fixes for web tool scenario
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BDCTBA/Boolean Disable Carbon Tax Border Adjustment.xlsx
+++ b/InputData/ctrl-settings/BDCTBA/Boolean Disable Carbon Tax Border Adjustment.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ctrl-settings\BDCTBA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\ctrl-settings\BDCTBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E7D65B-1630-457E-83C3-A8F9AD7513A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3963DB38-B518-427E-AB91-CBA3F11DC3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2910" yWindow="3165" windowWidth="18555" windowHeight="9120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BDCTBA" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -47,10 +47,10 @@
     <t>industries.</t>
   </si>
   <si>
-    <t>Diable Carbon Tax Border Adjustment</t>
-  </si>
-  <si>
     <t>By default, the EPS assumes carbon tax border adjustments do not apply across</t>
+  </si>
+  <si>
+    <t>Disable Carbon Tax Border Adjustment</t>
   </si>
 </sst>
 </file>
@@ -115,9 +115,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -155,9 +155,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -190,26 +190,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -242,26 +225,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -437,7 +403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -475,7 +441,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
@@ -496,15 +462,15 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>